<commit_message>
feat(sectorXmapping): sector X mapping revised and generalized, works with any energy scope layer
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_EnergyScope_BS.xlsx
+++ b/ConfigFiles/Config_EnergyScope_BS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-LINK\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA2EF08-BD67-415D-9ADD-A4D85F8AD10E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00465ADC-18DB-4A64-8479-CA724BEAEEF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="246">
   <si>
     <t>Default value</t>
   </si>
@@ -425,9 +425,6 @@
     <t>CPLEX path</t>
   </si>
   <si>
-    <t>Heat Demand</t>
-  </si>
-  <si>
     <t>Integer clustering</t>
   </si>
   <si>
@@ -764,9 +761,6 @@
     <t>Outputs/EnergyScope/Database/AvailabilityFactors/##/AF_2015_ES.csv</t>
   </si>
   <si>
-    <t>Outputs/EnergyScope/Database/HeatDemand/2015_ES_th.csv</t>
-  </si>
-  <si>
     <t>CPLEX Accuracy</t>
   </si>
   <si>
@@ -777,6 +771,9 @@
   </si>
   <si>
     <t>Agressive</t>
+  </si>
+  <si>
+    <t>Scaled outflows</t>
   </si>
 </sst>
 </file>
@@ -1527,8 +1524,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="F168" sqref="F168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1546,7 +1543,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -1594,7 +1591,7 @@
         <v>49</v>
       </c>
       <c r="B6" s="43" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C6" s="43"/>
       <c r="D6" s="43"/>
@@ -1677,7 +1674,7 @@
     </row>
     <row r="15" spans="1:8" s="35" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34"/>
@@ -1695,13 +1692,13 @@
     </row>
     <row r="17" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B17" s="27"/>
     </row>
     <row r="18" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B18" s="25"/>
     </row>
@@ -1721,7 +1718,7 @@
     <row r="32" spans="1:2" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B33" s="33"/>
       <c r="C33" s="34"/>
@@ -1739,7 +1736,7 @@
         <v>35</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D34" s="13"/>
       <c r="H34" s="1" t="s">
@@ -1797,10 +1794,10 @@
     </row>
     <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C39" s="42">
         <v>5.0000000000000001E-4</v>
@@ -1808,13 +1805,13 @@
     </row>
     <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B40" s="27" t="s">
         <v>59</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1834,7 +1831,7 @@
     <row r="55" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="56" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B56" s="33"/>
       <c r="C56" s="34"/>
@@ -1899,10 +1896,10 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B61" s="25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C61" s="4">
         <v>1</v>
@@ -1910,10 +1907,10 @@
     </row>
     <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B62" s="25" t="s">
         <v>192</v>
-      </c>
-      <c r="B62" s="25" t="s">
-        <v>193</v>
       </c>
       <c r="C62" s="4">
         <v>1</v>
@@ -1933,7 +1930,7 @@
     <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="75" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B75" s="33"/>
       <c r="C75" s="34"/>
@@ -1954,7 +1951,7 @@
         <v>59</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>63</v>
@@ -2011,7 +2008,7 @@
     <row r="97" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="98" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B98" s="33"/>
       <c r="C98" s="34"/>
@@ -2023,35 +2020,35 @@
     </row>
     <row r="99" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B99" s="27" t="s">
         <v>59</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B100" s="27" t="s">
         <v>59</v>
       </c>
       <c r="C100" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="H100" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="H100" s="1" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B101" s="27" t="s">
         <v>4</v>
@@ -2062,7 +2059,7 @@
     </row>
     <row r="102" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E102" s="25" t="s">
         <v>0</v>
@@ -2071,12 +2068,12 @@
         <v>0.5</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E103" s="25" t="s">
         <v>0</v>
@@ -2085,7 +2082,7 @@
         <v>0.5</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2113,7 +2110,7 @@
     </row>
     <row r="124" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B124" s="33"/>
       <c r="C124" s="34"/>
@@ -2131,7 +2128,7 @@
         <v>35</v>
       </c>
       <c r="C125" s="19" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D125" s="18" t="s">
         <v>87</v>
@@ -2140,7 +2137,7 @@
     </row>
     <row r="126" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B126" s="26" t="s">
         <v>35</v>
@@ -2180,13 +2177,13 @@
         <v>35</v>
       </c>
       <c r="C128" s="19" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D128" s="18" t="s">
         <v>87</v>
       </c>
       <c r="H128" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="129" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2197,7 +2194,7 @@
         <v>35</v>
       </c>
       <c r="C129" s="19" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D129" s="18" t="s">
         <v>87</v>
@@ -2283,21 +2280,19 @@
     </row>
     <row r="135" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>129</v>
+        <v>245</v>
       </c>
       <c r="B135" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="C135" s="19" t="s">
-        <v>242</v>
-      </c>
+      <c r="C135" s="19"/>
       <c r="D135" s="18" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="136" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B136" s="26" t="s">
         <v>35</v>
@@ -2310,7 +2305,7 @@
     </row>
     <row r="137" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B137" s="26" t="s">
         <v>35</v>
@@ -2322,7 +2317,7 @@
     </row>
     <row r="138" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B138" s="26" t="s">
         <v>35</v>
@@ -2331,7 +2326,7 @@
     </row>
     <row r="139" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B139" s="26" t="s">
         <v>35</v>
@@ -2340,7 +2335,7 @@
     </row>
     <row r="140" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B140" s="26" t="s">
         <v>35</v>
@@ -2349,7 +2344,7 @@
     </row>
     <row r="141" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B141" s="26" t="s">
         <v>35</v>
@@ -2358,7 +2353,7 @@
     </row>
     <row r="142" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B142" s="26" t="s">
         <v>35</v>
@@ -2367,7 +2362,7 @@
     </row>
     <row r="143" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B143" s="26" t="s">
         <v>35</v>
@@ -2399,7 +2394,7 @@
     <row r="160" spans="3:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="161" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B161" s="26" t="s">
         <v>35</v>
@@ -2408,7 +2403,7 @@
     </row>
     <row r="162" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B162" s="26" t="s">
         <v>35</v>
@@ -2417,7 +2412,7 @@
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C163" s="1"/>
       <c r="E163" s="25" t="s">
@@ -2427,12 +2422,12 @@
         <v>0</v>
       </c>
       <c r="H163" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E164" s="25" t="s">
         <v>0</v>
@@ -2441,13 +2436,13 @@
         <v>0.5</v>
       </c>
       <c r="H164" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="165" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="166" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="32" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B166" s="33"/>
       <c r="C166" s="34"/>
@@ -2477,7 +2472,7 @@
     </row>
     <row r="168" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B168" s="26" t="s">
         <v>35</v>
@@ -2490,12 +2485,12 @@
         <v>0</v>
       </c>
       <c r="F168" s="5">
-        <v>1001</v>
+        <v>110000</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B169" s="26" t="s">
         <v>35</v>
@@ -2508,15 +2503,15 @@
         <v>0</v>
       </c>
       <c r="F169" s="5">
-        <v>400</v>
+        <v>1500</v>
       </c>
       <c r="H169" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="170" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B170" s="26" t="s">
         <v>35</v>
@@ -2532,12 +2527,12 @@
         <v>0</v>
       </c>
       <c r="H170" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="171" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B171" s="26" t="s">
         <v>35</v>
@@ -2550,12 +2545,12 @@
         <v>0</v>
       </c>
       <c r="F171" s="5">
-        <v>1000</v>
+        <v>110000</v>
       </c>
     </row>
     <row r="172" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B172" s="26" t="s">
         <v>35</v>
@@ -2711,7 +2706,7 @@
     </row>
     <row r="188" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B188" s="26" t="s">
         <v>35</v>
@@ -2744,7 +2739,7 @@
     <row r="204" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="205" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C205" s="1"/>
       <c r="E205" s="25" t="s">
@@ -2754,12 +2749,12 @@
         <v>100000</v>
       </c>
       <c r="H205" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="206" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C206" s="1"/>
       <c r="E206" s="25" t="s">
@@ -2769,22 +2764,22 @@
         <v>1502</v>
       </c>
       <c r="H206" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C207" s="1"/>
       <c r="E207" s="25" t="s">
         <v>0</v>
       </c>
       <c r="F207" s="5">
-        <v>1500</v>
+        <v>120000</v>
       </c>
       <c r="H207" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="209" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2808,25 +2803,25 @@
     </row>
     <row r="225" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="36" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B225" s="28" t="s">
         <v>4</v>
       </c>
       <c r="C225" s="36" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D225" s="39" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E225" s="28" t="s">
         <v>4</v>
       </c>
       <c r="F225" s="36" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G225" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H225" s="37"/>
     </row>
@@ -2835,7 +2830,7 @@
         <v>50</v>
       </c>
       <c r="B226" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C226" s="4" t="b">
         <v>0</v>
@@ -2844,7 +2839,7 @@
         <v>0</v>
       </c>
       <c r="E226" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F226" s="4" t="b">
         <v>0</v>
@@ -2858,7 +2853,7 @@
         <v>51</v>
       </c>
       <c r="B227" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C227" s="4" t="b">
         <v>0</v>
@@ -2867,7 +2862,7 @@
         <v>0</v>
       </c>
       <c r="E227" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F227" s="4" t="b">
         <v>0</v>
@@ -2900,7 +2895,7 @@
     <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="44"/>
       <c r="B229" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C229" s="4" t="b">
         <v>0</v>
@@ -2921,7 +2916,7 @@
     <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="44"/>
       <c r="B230" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C230" s="4" t="b">
         <v>0</v>
@@ -2930,7 +2925,7 @@
         <v>0</v>
       </c>
       <c r="E230" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F230" s="4" t="b">
         <v>0</v>
@@ -2951,7 +2946,7 @@
         <v>0</v>
       </c>
       <c r="E231" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F231" s="4" t="b">
         <v>0</v>
@@ -2963,16 +2958,16 @@
     <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="44"/>
       <c r="B232" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C232" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D232" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E232" s="6" t="s">
         <v>152</v>
-      </c>
-      <c r="C232" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D232" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E232" s="6" t="s">
-        <v>153</v>
       </c>
       <c r="F232" s="4" t="b">
         <v>0</v>
@@ -3014,7 +3009,7 @@
         <v>0</v>
       </c>
       <c r="E234" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F234" s="4" t="b">
         <v>0</v>
@@ -3119,7 +3114,7 @@
         <v>0</v>
       </c>
       <c r="E239" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F239" s="4" t="b">
         <v>0</v>
@@ -3140,7 +3135,7 @@
         <v>1</v>
       </c>
       <c r="E240" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F240" s="4" t="b">
         <v>0</v>
@@ -3221,7 +3216,7 @@
         <v>0</v>
       </c>
       <c r="E244" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F244" s="4" t="b">
         <v>0</v>
@@ -3232,7 +3227,7 @@
     </row>
     <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="47" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B245" s="6" t="s">
         <v>10</v>
@@ -3244,7 +3239,7 @@
         <v>0</v>
       </c>
       <c r="E245" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F245" s="4" t="b">
         <v>0</v>
@@ -3256,7 +3251,7 @@
     <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="47"/>
       <c r="B246" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C246" s="4" t="b">
         <v>0</v>
@@ -3274,7 +3269,7 @@
         <v>0</v>
       </c>
       <c r="H246" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="247" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3288,7 +3283,7 @@
         <v>0</v>
       </c>
       <c r="E247" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F247" s="4" t="b">
         <v>0</v>
@@ -3406,7 +3401,7 @@
     <row r="297" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="298" spans="1:8" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A298" s="32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B298" s="33"/>
       <c r="C298" s="34"/>
@@ -3418,7 +3413,7 @@
     </row>
     <row r="299" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C299" s="28" t="s">
         <v>4</v>
@@ -3473,7 +3468,7 @@
     </row>
     <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C305" s="28" t="s">
         <v>4</v>
@@ -3490,7 +3485,7 @@
         <v>1</v>
       </c>
       <c r="E306" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F306" s="21" t="b">
         <v>1</v>
@@ -3504,7 +3499,7 @@
         <v>1</v>
       </c>
       <c r="E307" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F307" s="21" t="b">
         <v>1</v>
@@ -3518,7 +3513,7 @@
         <v>1</v>
       </c>
       <c r="E308" s="22" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F308" s="21" t="b">
         <v>1</v>
@@ -3532,7 +3527,7 @@
         <v>0</v>
       </c>
       <c r="E309" s="22" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F309" s="21" t="b">
         <v>1</v>
@@ -3546,7 +3541,7 @@
         <v>1</v>
       </c>
       <c r="E310" s="22" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F310" s="21" t="b">
         <v>1</v>
@@ -3560,7 +3555,7 @@
         <v>1</v>
       </c>
       <c r="E311" s="22" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F311" s="21" t="b">
         <v>1</v>
@@ -3574,7 +3569,7 @@
         <v>0</v>
       </c>
       <c r="E312" s="22" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F312" s="21" t="b">
         <v>1</v>
@@ -3588,7 +3583,7 @@
         <v>0</v>
       </c>
       <c r="E313" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F313" s="21" t="b">
         <v>0</v>
@@ -3602,7 +3597,7 @@
         <v>0</v>
       </c>
       <c r="E314" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F314" s="21" t="b">
         <v>0</v>
@@ -3616,7 +3611,7 @@
         <v>0</v>
       </c>
       <c r="E315" s="22" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F315" s="21" t="b">
         <v>0</v>
@@ -3630,7 +3625,7 @@
         <v>1</v>
       </c>
       <c r="E316" s="22" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F316" s="21" t="b">
         <v>0</v>
@@ -3644,7 +3639,7 @@
         <v>1</v>
       </c>
       <c r="E317" s="22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F317" s="21" t="b">
         <v>0</v>
@@ -3658,7 +3653,7 @@
         <v>1</v>
       </c>
       <c r="E318" s="22" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F318" s="21" t="b">
         <v>0</v>
@@ -3672,7 +3667,7 @@
         <v>0</v>
       </c>
       <c r="E319" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F319" s="21" t="b">
         <v>0</v>
@@ -3686,7 +3681,7 @@
         <v>0</v>
       </c>
       <c r="E320" s="22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F320" s="21" t="b">
         <v>0</v>
@@ -3694,13 +3689,13 @@
     </row>
     <row r="321" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B321" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="C321" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E321" s="22" t="s">
         <v>224</v>
-      </c>
-      <c r="C321" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E321" s="22" t="s">
-        <v>225</v>
       </c>
       <c r="F321" s="21" t="b">
         <v>0</v>
@@ -3708,7 +3703,7 @@
     </row>
     <row r="322" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E322" s="22" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F322" s="21" t="b">
         <v>0</v>
@@ -3716,7 +3711,7 @@
     </row>
     <row r="325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.25">
@@ -3790,7 +3785,7 @@
       <formula2>73051</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Historical interconnection flows" prompt="Historical flows" sqref="C132" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F171:F172 F168 F181:F188" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F171:F172 F181:F188 F168" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the demand curves of all the zones by the provided factor" sqref="C275" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the wind generation curves of all the zones by the provided factor" sqref="C276" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the PV generation curves of all the zones by the provided factor" sqref="C277" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
@@ -3924,10 +3919,10 @@
         <v>79</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3935,7 +3930,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C2" t="s">
         <v>58</v>
@@ -3944,10 +3939,10 @@
         <v>82</v>
       </c>
       <c r="E2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3958,16 +3953,16 @@
         <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D3" t="s">
         <v>83</v>
       </c>
       <c r="E3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3975,21 +3970,21 @@
         <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D4" t="s">
         <v>80</v>
       </c>
       <c r="E4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D5" t="s">
         <v>81</v>
@@ -3997,7 +3992,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(plots): a new plot.py script to summarize the results
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_EnergyScope_BS.xlsx
+++ b/ConfigFiles/Config_EnergyScope_BS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-LINK\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00465ADC-18DB-4A64-8479-CA724BEAEEF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB308A30-A6BA-4D9E-AE34-91F80BF9502B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1525,7 +1525,7 @@
   <dimension ref="A1:H330"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="F168" sqref="F168"/>
+      <selection activeCell="F180" sqref="F180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2485,7 +2485,7 @@
         <v>0</v>
       </c>
       <c r="F168" s="5">
-        <v>110000</v>
+        <v>11000</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
@@ -2503,7 +2503,7 @@
         <v>0</v>
       </c>
       <c r="F169" s="5">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="H169" s="1" t="s">
         <v>174</v>
@@ -2545,7 +2545,7 @@
         <v>0</v>
       </c>
       <c r="F171" s="5">
-        <v>110000</v>
+        <v>11000</v>
       </c>
     </row>
     <row r="172" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2746,7 +2746,7 @@
         <v>0</v>
       </c>
       <c r="F205" s="24">
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="H205" s="1" t="s">
         <v>189</v>
@@ -2761,7 +2761,7 @@
         <v>0</v>
       </c>
       <c r="F206" s="5">
-        <v>1502</v>
+        <v>3002</v>
       </c>
       <c r="H206" s="1" t="s">
         <v>145</v>
@@ -2776,7 +2776,7 @@
         <v>0</v>
       </c>
       <c r="F207" s="5">
-        <v>120000</v>
+        <v>12000</v>
       </c>
       <c r="H207" s="1" t="s">
         <v>146</v>

</xml_diff>